<commit_message>
Adding details to the excel
</commit_message>
<xml_diff>
--- a/model_details.xlsx
+++ b/model_details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venku/Documents/PyCharmProjects/home_security_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B575F0-C164-F84B-BF64-13E551074229}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57474213-A3CF-6C4B-BBC2-8A0AC7D87428}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4041E564-9E2B-1947-9043-62B7FC74195F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
   <si>
     <t>Train</t>
   </si>
@@ -39,6 +39,9 @@
     <t>Test</t>
   </si>
   <si>
+    <t xml:space="preserve">              precision    recall  f1-score   support</t>
+  </si>
+  <si>
     <t>Rush</t>
   </si>
   <si>
@@ -85,6 +88,36 @@
   </si>
   <si>
     <t>Latent Dirichlet Allocation</t>
+  </si>
+  <si>
+    <t>[[19  6  2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0 26  0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [ 0  2 28]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           0       1.00      0.70      0.83        27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           1       0.76      1.00      0.87        26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">           2       0.93      0.93      0.93        30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    accuracy                           0.88        83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   macro avg       0.90      0.88      0.88        83</t>
+  </si>
+  <si>
+    <t>weighted avg       0.90      0.88      0.88        83</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -447,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9D681D-00C4-F146-AB30-D8BF52E00CA4}">
-  <dimension ref="B2:W71"/>
+  <dimension ref="B2:W91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -473,7 +506,7 @@
     </row>
     <row r="3" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -497,29 +530,29 @@
     </row>
     <row r="5" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="N5" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -529,7 +562,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
@@ -563,7 +596,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -595,7 +628,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -633,19 +666,19 @@
     <row r="11" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -713,7 +746,7 @@
     <row r="15" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -729,7 +762,7 @@
     <row r="16" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="1">
         <v>0.9</v>
@@ -749,7 +782,7 @@
     <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1">
         <v>0.91</v>
@@ -788,7 +821,7 @@
     </row>
     <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -806,17 +839,17 @@
     </row>
     <row r="23" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -825,7 +858,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D24" s="1">
         <v>21</v>
@@ -843,7 +876,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -861,7 +894,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
@@ -893,19 +926,19 @@
     <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.25">
@@ -965,7 +998,7 @@
     <row r="33" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -979,7 +1012,7 @@
     <row r="34" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D34" s="1">
         <v>0.82</v>
@@ -997,7 +1030,7 @@
     <row r="35" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D35" s="1">
         <v>0.82</v>
@@ -1014,7 +1047,7 @@
     </row>
     <row r="39" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1032,17 +1065,17 @@
     </row>
     <row r="41" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F41" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1051,7 +1084,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1">
         <v>21</v>
@@ -1069,7 +1102,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D43" s="1">
         <v>2</v>
@@ -1087,7 +1120,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
@@ -1119,19 +1152,19 @@
     <row r="47" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="21" x14ac:dyDescent="0.25">
@@ -1191,7 +1224,7 @@
     <row r="51" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1205,7 +1238,7 @@
     <row r="52" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D52" s="1">
         <v>0.82</v>
@@ -1223,7 +1256,7 @@
     <row r="53" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D53" s="1">
         <v>0.82</v>
@@ -1240,7 +1273,7 @@
     </row>
     <row r="57" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1258,17 +1291,17 @@
     </row>
     <row r="59" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="F59" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -1277,7 +1310,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D60" s="1">
         <v>20</v>
@@ -1295,7 +1328,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -1313,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D62" s="1">
         <v>6</v>
@@ -1345,19 +1378,19 @@
     <row r="65" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="21" x14ac:dyDescent="0.25">
@@ -1417,7 +1450,7 @@
     <row r="69" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -1431,7 +1464,7 @@
     <row r="70" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D70" s="1">
         <v>0.82</v>
@@ -1449,7 +1482,7 @@
     <row r="71" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D71" s="1">
         <v>0.82</v>
@@ -1464,12 +1497,275 @@
         <v>83</v>
       </c>
     </row>
+    <row r="74" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="2"/>
+      <c r="G74" s="2"/>
+    </row>
+    <row r="75" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+    </row>
+    <row r="76" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G76" s="1"/>
+    </row>
+    <row r="77" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
+        <v>0</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="1">
+        <v>19</v>
+      </c>
+      <c r="E77" s="1">
+        <v>6</v>
+      </c>
+      <c r="F77" s="1">
+        <v>2</v>
+      </c>
+      <c r="G77" s="1"/>
+    </row>
+    <row r="78" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
+        <v>1</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="1">
+        <v>0</v>
+      </c>
+      <c r="E78" s="1">
+        <v>26</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1"/>
+    </row>
+    <row r="79" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
+        <v>2</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>2</v>
+      </c>
+      <c r="F79" s="1">
+        <v>28</v>
+      </c>
+      <c r="G79" s="1"/>
+    </row>
+    <row r="80" spans="2:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+    </row>
+    <row r="81" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+    </row>
+    <row r="82" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B82" s="1"/>
+      <c r="C82" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P82" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="83" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B83" s="1"/>
+      <c r="C83" s="1">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1">
+        <v>1</v>
+      </c>
+      <c r="E83" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="F83" s="1">
+        <v>0.83</v>
+      </c>
+      <c r="G83" s="1">
+        <v>27</v>
+      </c>
+      <c r="P83" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="84" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B84" s="1"/>
+      <c r="C84" s="1">
+        <v>1</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0.76</v>
+      </c>
+      <c r="E84" s="1">
+        <v>1</v>
+      </c>
+      <c r="F84" s="1">
+        <v>0.87</v>
+      </c>
+      <c r="G84" s="1">
+        <v>26</v>
+      </c>
+      <c r="P84" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B85" s="1"/>
+      <c r="C85" s="1">
+        <v>2</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="E85" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="F85" s="1">
+        <v>0.93</v>
+      </c>
+      <c r="G85" s="1">
+        <v>30</v>
+      </c>
+      <c r="P85" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B86" s="1"/>
+      <c r="C86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G86" s="1">
+        <v>83</v>
+      </c>
+      <c r="P86" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="87" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B87" s="1"/>
+      <c r="C87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E87" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F87" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G87" s="1">
+        <v>83</v>
+      </c>
+      <c r="P87" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="88" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="B88" s="1"/>
+      <c r="C88" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="E88" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="F88" s="1">
+        <v>0.88</v>
+      </c>
+      <c r="G88" s="1">
+        <v>83</v>
+      </c>
+      <c r="P88" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P89" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P90" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="P91" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B39:G39"/>
     <mergeCell ref="B57:G57"/>
+    <mergeCell ref="B74:G74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Adding readme file on how to run the code.
</commit_message>
<xml_diff>
--- a/model_details.xlsx
+++ b/model_details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venku/Documents/PyCharmProjects/home_security_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57474213-A3CF-6C4B-BBC2-8A0AC7D87428}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A2C36F3-8198-AF41-80A4-96CB94589CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{4041E564-9E2B-1947-9043-62B7FC74195F}"/>
+    <workbookView xWindow="600" yWindow="460" windowWidth="28200" windowHeight="17540" xr2:uid="{4041E564-9E2B-1947-9043-62B7FC74195F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="19">
   <si>
     <t>Train</t>
   </si>
@@ -39,9 +39,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t xml:space="preserve">              precision    recall  f1-score   support</t>
-  </si>
-  <si>
     <t>Rush</t>
   </si>
   <si>
@@ -88,33 +85,6 @@
   </si>
   <si>
     <t>Latent Dirichlet Allocation</t>
-  </si>
-  <si>
-    <t>[[19  6  2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 0 26  0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> [ 0  2 28]]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           0       1.00      0.70      0.83        27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           1       0.76      1.00      0.87        26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">           2       0.93      0.93      0.93        30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    accuracy                           0.88        83</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   macro avg       0.90      0.88      0.88        83</t>
-  </si>
-  <si>
-    <t>weighted avg       0.90      0.88      0.88        83</t>
   </si>
   <si>
     <t>SGD</t>
@@ -480,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9D681D-00C4-F146-AB30-D8BF52E00CA4}">
-  <dimension ref="B2:W91"/>
+  <dimension ref="B2:W88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="I91" sqref="I91"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="P81" sqref="P81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +476,7 @@
     </row>
     <row r="3" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -530,29 +500,29 @@
     </row>
     <row r="5" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="N5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="P5" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
@@ -562,7 +532,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" s="1">
         <v>24</v>
@@ -596,7 +566,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -628,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D8" s="1">
         <v>3</v>
@@ -666,19 +636,19 @@
     <row r="11" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -746,7 +716,7 @@
     <row r="15" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -762,7 +732,7 @@
     <row r="16" spans="2:23" ht="21" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D16" s="1">
         <v>0.9</v>
@@ -782,7 +752,7 @@
     <row r="17" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17" s="1">
         <v>0.91</v>
@@ -821,7 +791,7 @@
     </row>
     <row r="21" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -839,17 +809,17 @@
     </row>
     <row r="23" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" s="1"/>
     </row>
@@ -858,7 +828,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D24" s="1">
         <v>21</v>
@@ -876,7 +846,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1">
         <v>2</v>
@@ -894,7 +864,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1">
         <v>3</v>
@@ -926,19 +896,19 @@
     <row r="29" spans="2:9" ht="21" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G29" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="30" spans="2:9" ht="21" x14ac:dyDescent="0.25">
@@ -998,7 +968,7 @@
     <row r="33" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -1012,7 +982,7 @@
     <row r="34" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" s="1">
         <v>0.82</v>
@@ -1030,7 +1000,7 @@
     <row r="35" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D35" s="1">
         <v>0.82</v>
@@ -1047,7 +1017,7 @@
     </row>
     <row r="39" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1065,17 +1035,17 @@
     </row>
     <row r="41" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G41" s="1"/>
     </row>
@@ -1084,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D42" s="1">
         <v>21</v>
@@ -1102,7 +1072,7 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D43" s="1">
         <v>2</v>
@@ -1120,7 +1090,7 @@
         <v>2</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D44" s="1">
         <v>3</v>
@@ -1152,19 +1122,19 @@
     <row r="47" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B47" s="1"/>
       <c r="C47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="G47" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="21" x14ac:dyDescent="0.25">
@@ -1224,7 +1194,7 @@
     <row r="51" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -1238,7 +1208,7 @@
     <row r="52" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D52" s="1">
         <v>0.82</v>
@@ -1256,7 +1226,7 @@
     <row r="53" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D53" s="1">
         <v>0.82</v>
@@ -1273,7 +1243,7 @@
     </row>
     <row r="57" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B57" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
@@ -1291,17 +1261,17 @@
     </row>
     <row r="59" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G59" s="1"/>
     </row>
@@ -1310,7 +1280,7 @@
         <v>0</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D60" s="1">
         <v>20</v>
@@ -1328,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D61" s="1">
         <v>1</v>
@@ -1346,7 +1316,7 @@
         <v>2</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D62" s="1">
         <v>6</v>
@@ -1378,19 +1348,19 @@
     <row r="65" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B65" s="1"/>
       <c r="C65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D65" s="1" t="s">
+      <c r="E65" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E65" s="1" t="s">
+      <c r="F65" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F65" s="1" t="s">
+      <c r="G65" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="G65" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="66" spans="2:7" ht="21" x14ac:dyDescent="0.25">
@@ -1450,7 +1420,7 @@
     <row r="69" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B69" s="1"/>
       <c r="C69" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -1464,7 +1434,7 @@
     <row r="70" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B70" s="1"/>
       <c r="C70" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70" s="1">
         <v>0.82</v>
@@ -1482,7 +1452,7 @@
     <row r="71" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B71" s="1"/>
       <c r="C71" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D71" s="1">
         <v>0.82</v>
@@ -1499,7 +1469,7 @@
     </row>
     <row r="74" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B74" s="2" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
@@ -1517,17 +1487,17 @@
     </row>
     <row r="76" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G76" s="1"/>
     </row>
@@ -1536,7 +1506,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D77" s="1">
         <v>19</v>
@@ -1554,7 +1524,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -1572,7 +1542,7 @@
         <v>2</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -1593,7 +1563,7 @@
       <c r="F80" s="1"/>
       <c r="G80" s="1"/>
     </row>
-    <row r="81" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -1601,28 +1571,25 @@
       <c r="F81" s="1"/>
       <c r="G81" s="1"/>
     </row>
-    <row r="82" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B82" s="1"/>
       <c r="C82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F82" s="1" t="s">
+      <c r="G82" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G82" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="P82" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="83" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B83" s="1"/>
       <c r="C83" s="1">
         <v>0</v>
@@ -1639,11 +1606,8 @@
       <c r="G83" s="1">
         <v>27</v>
       </c>
-      <c r="P83" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="84" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B84" s="1"/>
       <c r="C84" s="1">
         <v>1</v>
@@ -1660,11 +1624,8 @@
       <c r="G84" s="1">
         <v>26</v>
       </c>
-      <c r="P84" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="85" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B85" s="1"/>
       <c r="C85" s="1">
         <v>2</v>
@@ -1681,14 +1642,11 @@
       <c r="G85" s="1">
         <v>30</v>
       </c>
-      <c r="P85" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="86" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B86" s="1"/>
       <c r="C86" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
@@ -1698,14 +1656,11 @@
       <c r="G86" s="1">
         <v>83</v>
       </c>
-      <c r="P86" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="87" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B87" s="1"/>
       <c r="C87" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D87" s="1">
         <v>0.9</v>
@@ -1719,14 +1674,11 @@
       <c r="G87" s="1">
         <v>83</v>
       </c>
-      <c r="P87" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="88" spans="2:16" ht="21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="2:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B88" s="1"/>
       <c r="C88" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D88" s="1">
         <v>0.9</v>
@@ -1739,24 +1691,6 @@
       </c>
       <c r="G88" s="1">
         <v>83</v>
-      </c>
-      <c r="P88" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="89" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P89" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="90" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P90" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="91" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="P91" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>